<commit_message>
cambiado a resolución anterior
</commit_message>
<xml_diff>
--- a/src/main/resources/TablasBingo.xlsx
+++ b/src/main/resources/TablasBingo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3491" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3929" uniqueCount="11">
   <si>
     <t xml:space="preserve">Nº 1</t>
   </si>
@@ -62,7 +62,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="59">
+  <fonts count="65">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -101,6 +101,33 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="20.0"/>
+    </font>
+    <font>
+      <name val="Cambria"/>
+      <sz val="18.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="20.0"/>
+    </font>
+    <font>
+      <name val="Cambria"/>
+      <sz val="18.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="20.0"/>
+    </font>
+    <font>
+      <name val="Cambria"/>
+      <sz val="18.0"/>
+      <i val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -399,7 +426,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3401">
+  <cellXfs count="3833">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -10606,6 +10633,1302 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="58" fillId="5" borderId="0" xfId="0" applyFont="true" applyAlignment="true" applyFill="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="5" borderId="0" xfId="0" applyFont="true" applyAlignment="true" applyFill="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="5" borderId="0" xfId="0" applyFont="true" applyAlignment="true" applyFill="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="5" borderId="0" xfId="0" applyFont="true" applyAlignment="true" applyFill="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -10803,499 +12126,499 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3400" t="s">
+      <c r="A1" s="3832" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3400"/>
-      <c r="C1" s="3400"/>
-      <c r="D1" s="3400" t="s">
+      <c r="B1" s="3832"/>
+      <c r="C1" s="3832"/>
+      <c r="D1" s="3832" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3400" t="s">
+      <c r="E1" s="3832" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3399" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="B2" s="3399" t="n">
-        <v>17.0</v>
-      </c>
-      <c r="C2" s="3399" t="n">
-        <v>41.0</v>
-      </c>
-      <c r="D2" s="3399" t="n">
+      <c r="A2" s="3831" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B2" s="3831" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="C2" s="3831" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="D2" s="3831" t="n">
         <v>58.0</v>
       </c>
-      <c r="E2" s="3399" t="n">
-        <v>61.0</v>
+      <c r="E2" s="3831" t="n">
+        <v>64.0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3399" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B3" s="3399" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="C3" s="3399" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="D3" s="3399" t="n">
-        <v>59.0</v>
-      </c>
-      <c r="E3" s="3399" t="n">
-        <v>66.0</v>
-      </c>
-      <c r="F3" s="3267" t="s">
+      <c r="A3" s="3831" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B3" s="3831" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="C3" s="3831" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="D3" s="3831" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="E3" s="3831" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="F3" s="3699" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3399" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B4" s="3399" t="n">
-        <v>25.0</v>
-      </c>
-      <c r="C4" s="3270" t="s">
+      <c r="A4" s="3831" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B4" s="3831" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="C4" s="3702" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3399" t="n">
-        <v>52.0</v>
-      </c>
-      <c r="E4" s="3399" t="n">
-        <v>68.0</v>
+      <c r="D4" s="3831" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="E4" s="3831" t="n">
+        <v>74.0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3399" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="B5" s="3399" t="n">
+      <c r="A5" s="3831" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B5" s="3831" t="n">
         <v>28.0</v>
       </c>
-      <c r="C5" s="3399" t="n">
-        <v>35.0</v>
-      </c>
-      <c r="D5" s="3399" t="n">
-        <v>47.0</v>
-      </c>
-      <c r="E5" s="3399" t="n">
-        <v>62.0</v>
+      <c r="C5" s="3831" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="D5" s="3831" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="E5" s="3831" t="n">
+        <v>75.0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3399" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="B6" s="3399" t="n">
-        <v>16.0</v>
-      </c>
-      <c r="C6" s="3399" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="D6" s="3399" t="n">
-        <v>57.0</v>
-      </c>
-      <c r="E6" s="3399" t="n">
-        <v>67.0</v>
+      <c r="A6" s="3831" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B6" s="3831" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="C6" s="3831" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="D6" s="3831" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="E6" s="3831" t="n">
+        <v>71.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s" s="3400">
+      <c r="A7" t="s" s="3832">
         <v>7</v>
       </c>
-      <c r="B7" s="3400" t="s">
+      <c r="B7" s="3832" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="3400" t="s">
+      <c r="C7" s="3832" t="s">
         <v>3</v>
       </c>
-      <c r="D7" t="s" s="3400">
+      <c r="D7" t="s" s="3832">
         <v>5</v>
       </c>
-      <c r="E7" t="s" s="3400">
+      <c r="E7" t="s" s="3832">
         <v>6</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n" s="3399">
-        <v>12.0</v>
-      </c>
-      <c r="B8" t="n" s="3399">
+      <c r="A8" t="n" s="3831">
+        <v>8.0</v>
+      </c>
+      <c r="B8" t="n" s="3831">
         <v>21.0</v>
       </c>
-      <c r="C8" t="n" s="3399">
-        <v>34.0</v>
-      </c>
-      <c r="D8" t="n" s="3399">
-        <v>50.0</v>
-      </c>
-      <c r="E8" t="n" s="3399">
-        <v>68.0</v>
+      <c r="C8" t="n" s="3831">
+        <v>33.0</v>
+      </c>
+      <c r="D8" t="n" s="3831">
+        <v>59.0</v>
+      </c>
+      <c r="E8" t="n" s="3831">
+        <v>62.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n" s="3399">
-        <v>7.0</v>
-      </c>
-      <c r="B9" t="n" s="3399">
-        <v>25.0</v>
-      </c>
-      <c r="C9" t="n" s="3399">
-        <v>36.0</v>
-      </c>
-      <c r="D9" t="n" s="3399">
-        <v>54.0</v>
-      </c>
-      <c r="E9" t="n" s="3399">
-        <v>61.0</v>
+      <c r="A9" t="n" s="3831">
+        <v>2.0</v>
+      </c>
+      <c r="B9" t="n" s="3831">
+        <v>18.0</v>
+      </c>
+      <c r="C9" t="n" s="3831">
+        <v>41.0</v>
+      </c>
+      <c r="D9" t="n" s="3831">
+        <v>57.0</v>
+      </c>
+      <c r="E9" t="n" s="3831">
+        <v>70.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n" s="3399">
-        <v>13.0</v>
-      </c>
-      <c r="B10" t="n" s="3399">
-        <v>27.0</v>
-      </c>
-      <c r="D10" t="n" s="3399">
-        <v>59.0</v>
-      </c>
-      <c r="E10" t="n" s="3399">
-        <v>74.0</v>
+      <c r="A10" t="n" s="3831">
+        <v>1.0</v>
+      </c>
+      <c r="B10" t="n" s="3831">
+        <v>30.0</v>
+      </c>
+      <c r="D10" t="n" s="3831">
+        <v>58.0</v>
+      </c>
+      <c r="E10" t="n" s="3831">
+        <v>61.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n" s="3399">
-        <v>15.0</v>
-      </c>
-      <c r="B11" t="n" s="3399">
-        <v>23.0</v>
-      </c>
-      <c r="C11" t="n" s="3399">
-        <v>40.0</v>
-      </c>
-      <c r="D11" t="n" s="3399">
-        <v>52.0</v>
-      </c>
-      <c r="E11" t="n" s="3399">
-        <v>75.0</v>
+      <c r="A11" t="n" s="3831">
+        <v>4.0</v>
+      </c>
+      <c r="B11" t="n" s="3831">
+        <v>27.0</v>
+      </c>
+      <c r="C11" t="n" s="3831">
+        <v>36.0</v>
+      </c>
+      <c r="D11" t="n" s="3831">
+        <v>50.0</v>
+      </c>
+      <c r="E11" t="n" s="3831">
+        <v>67.0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n" s="3399">
+      <c r="A12" t="n" s="3831">
         <v>10.0</v>
       </c>
-      <c r="B12" t="n" s="3399">
-        <v>22.0</v>
-      </c>
-      <c r="C12" t="n" s="3399">
-        <v>38.0</v>
-      </c>
-      <c r="D12" t="n" s="3399">
+      <c r="B12" t="n" s="3831">
+        <v>28.0</v>
+      </c>
+      <c r="C12" t="n" s="3831">
+        <v>44.0</v>
+      </c>
+      <c r="D12" t="n" s="3831">
         <v>55.0</v>
       </c>
-      <c r="E12" t="n" s="3399">
-        <v>73.0</v>
+      <c r="E12" t="n" s="3831">
+        <v>71.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s" s="3400">
-        <v>8</v>
-      </c>
-      <c r="B13" s="3400" t="s">
+      <c r="A13" t="s" s="3744">
         <v>3</v>
       </c>
-      <c r="C13" s="3400" t="s">
+      <c r="B13" s="3745" t="s">
         <v>3</v>
       </c>
-      <c r="D13" t="s" s="3400">
-        <v>5</v>
-      </c>
-      <c r="E13" t="s" s="3400">
-        <v>6</v>
+      <c r="C13" s="3746" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s" s="3747">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s" s="3748">
+        <v>3</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n" s="3399">
-        <v>10.0</v>
-      </c>
-      <c r="B14" t="n" s="3399">
-        <v>30.0</v>
-      </c>
-      <c r="C14" t="n" s="3399">
-        <v>33.0</v>
-      </c>
-      <c r="D14" t="n" s="3399">
-        <v>56.0</v>
-      </c>
-      <c r="E14" t="n" s="3399">
-        <v>63.0</v>
+      <c r="A14" t="s" s="3749">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s" s="3750">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s" s="3751">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s" s="3752">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s" s="3753">
+        <v>3</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n" s="3399">
-        <v>5.0</v>
-      </c>
-      <c r="B15" t="n" s="3399">
-        <v>27.0</v>
-      </c>
-      <c r="C15" t="n" s="3399">
-        <v>35.0</v>
-      </c>
-      <c r="D15" t="n" s="3399">
-        <v>51.0</v>
-      </c>
-      <c r="E15" t="n" s="3399">
-        <v>73.0</v>
+      <c r="A15" t="s" s="3754">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s" s="3755">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s" s="3756">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s" s="3757">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s" s="3758">
+        <v>3</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n" s="3399">
-        <v>11.0</v>
-      </c>
-      <c r="B16" t="n" s="3399">
-        <v>18.0</v>
-      </c>
-      <c r="D16" t="n" s="3399">
-        <v>52.0</v>
-      </c>
-      <c r="E16" t="n" s="3399">
-        <v>61.0</v>
+      <c r="A16" t="s" s="3759">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s" s="3760">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s" s="3761">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s" s="3762">
+        <v>3</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n" s="3399">
-        <v>1.0</v>
-      </c>
-      <c r="B17" t="n" s="3399">
-        <v>25.0</v>
-      </c>
-      <c r="C17" t="n" s="3399">
-        <v>43.0</v>
-      </c>
-      <c r="D17" t="n" s="3399">
-        <v>55.0</v>
-      </c>
-      <c r="E17" t="n" s="3399">
-        <v>69.0</v>
+      <c r="A17" t="s" s="3763">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s" s="3764">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s" s="3765">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s" s="3766">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s" s="3767">
+        <v>3</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n" s="3399">
-        <v>7.0</v>
-      </c>
-      <c r="B18" t="n" s="3399">
-        <v>20.0</v>
-      </c>
-      <c r="C18" t="n" s="3399">
-        <v>34.0</v>
-      </c>
-      <c r="D18" t="n" s="3399">
-        <v>46.0</v>
-      </c>
-      <c r="E18" t="n" s="3399">
-        <v>75.0</v>
+      <c r="A18" t="s" s="3768">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s" s="3769">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s" s="3770">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s" s="3771">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s" s="3772">
+        <v>3</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s" s="3341">
+      <c r="A19" t="s" s="3773">
         <v>3</v>
       </c>
-      <c r="B19" s="3342" t="s">
+      <c r="B19" s="3774" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="3343" t="s">
+      <c r="C19" s="3775" t="s">
         <v>3</v>
       </c>
-      <c r="D19" t="s" s="3344">
+      <c r="D19" t="s" s="3776">
         <v>3</v>
       </c>
-      <c r="E19" t="s" s="3345">
+      <c r="E19" t="s" s="3777">
         <v>3</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s" s="3346">
+      <c r="A20" t="s" s="3778">
         <v>3</v>
       </c>
-      <c r="B20" t="s" s="3347">
+      <c r="B20" t="s" s="3779">
         <v>3</v>
       </c>
-      <c r="C20" t="s" s="3348">
+      <c r="C20" t="s" s="3780">
         <v>3</v>
       </c>
-      <c r="D20" t="s" s="3349">
+      <c r="D20" t="s" s="3781">
         <v>3</v>
       </c>
-      <c r="E20" t="s" s="3350">
+      <c r="E20" t="s" s="3782">
         <v>3</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s" s="3351">
+      <c r="A21" t="s" s="3783">
         <v>3</v>
       </c>
-      <c r="B21" t="s" s="3352">
+      <c r="B21" t="s" s="3784">
         <v>3</v>
       </c>
-      <c r="C21" t="s" s="3353">
+      <c r="C21" t="s" s="3785">
         <v>3</v>
       </c>
-      <c r="D21" t="s" s="3354">
+      <c r="D21" t="s" s="3786">
         <v>3</v>
       </c>
-      <c r="E21" t="s" s="3355">
+      <c r="E21" t="s" s="3787">
         <v>3</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s" s="3356">
+      <c r="A22" t="s" s="3788">
         <v>3</v>
       </c>
-      <c r="B22" t="s" s="3357">
+      <c r="B22" t="s" s="3789">
         <v>3</v>
       </c>
-      <c r="D22" t="s" s="3358">
+      <c r="D22" t="s" s="3790">
         <v>3</v>
       </c>
-      <c r="E22" t="s" s="3359">
+      <c r="E22" t="s" s="3791">
         <v>3</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s" s="3360">
+      <c r="A23" t="s" s="3792">
         <v>3</v>
       </c>
-      <c r="B23" t="s" s="3361">
+      <c r="B23" t="s" s="3793">
         <v>3</v>
       </c>
-      <c r="C23" t="s" s="3362">
+      <c r="C23" t="s" s="3794">
         <v>3</v>
       </c>
-      <c r="D23" t="s" s="3363">
+      <c r="D23" t="s" s="3795">
         <v>3</v>
       </c>
-      <c r="E23" t="s" s="3364">
+      <c r="E23" t="s" s="3796">
         <v>3</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s" s="3365">
+      <c r="A24" t="s" s="3797">
         <v>3</v>
       </c>
-      <c r="B24" t="s" s="3366">
+      <c r="B24" t="s" s="3798">
         <v>3</v>
       </c>
-      <c r="C24" t="s" s="3367">
+      <c r="C24" t="s" s="3799">
         <v>3</v>
       </c>
-      <c r="D24" t="s" s="3368">
+      <c r="D24" t="s" s="3800">
         <v>3</v>
       </c>
-      <c r="E24" t="s" s="3369">
+      <c r="E24" t="s" s="3801">
         <v>3</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s" s="3370">
+      <c r="A25" t="s" s="3802">
         <v>3</v>
       </c>
-      <c r="B25" s="3371" t="s">
+      <c r="B25" s="3803" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="3372" t="s">
+      <c r="C25" s="3804" t="s">
         <v>3</v>
       </c>
-      <c r="D25" t="s" s="3373">
+      <c r="D25" t="s" s="3805">
         <v>3</v>
       </c>
-      <c r="E25" t="s" s="3374">
+      <c r="E25" t="s" s="3806">
         <v>3</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s" s="3375">
+      <c r="A26" t="s" s="3807">
         <v>3</v>
       </c>
-      <c r="B26" t="s" s="3376">
+      <c r="B26" t="s" s="3808">
         <v>3</v>
       </c>
-      <c r="C26" t="s" s="3377">
+      <c r="C26" t="s" s="3809">
         <v>3</v>
       </c>
-      <c r="D26" t="s" s="3378">
+      <c r="D26" t="s" s="3810">
         <v>3</v>
       </c>
-      <c r="E26" t="s" s="3379">
+      <c r="E26" t="s" s="3811">
         <v>3</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s" s="3380">
+      <c r="A27" t="s" s="3812">
         <v>3</v>
       </c>
-      <c r="B27" t="s" s="3381">
+      <c r="B27" t="s" s="3813">
         <v>3</v>
       </c>
-      <c r="C27" t="s" s="3382">
+      <c r="C27" t="s" s="3814">
         <v>3</v>
       </c>
-      <c r="D27" t="s" s="3383">
+      <c r="D27" t="s" s="3815">
         <v>3</v>
       </c>
-      <c r="E27" t="s" s="3384">
+      <c r="E27" t="s" s="3816">
         <v>3</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="s" s="3385">
+      <c r="A28" t="s" s="3817">
         <v>3</v>
       </c>
-      <c r="B28" t="s" s="3386">
+      <c r="B28" t="s" s="3818">
         <v>3</v>
       </c>
-      <c r="D28" t="s" s="3387">
+      <c r="D28" t="s" s="3819">
         <v>3</v>
       </c>
-      <c r="E28" t="s" s="3388">
+      <c r="E28" t="s" s="3820">
         <v>3</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="s" s="3389">
+      <c r="A29" t="s" s="3821">
         <v>3</v>
       </c>
-      <c r="B29" t="s" s="3390">
+      <c r="B29" t="s" s="3822">
         <v>3</v>
       </c>
-      <c r="C29" t="s" s="3391">
+      <c r="C29" t="s" s="3823">
         <v>3</v>
       </c>
-      <c r="D29" t="s" s="3392">
+      <c r="D29" t="s" s="3824">
         <v>3</v>
       </c>
-      <c r="E29" t="s" s="3393">
+      <c r="E29" t="s" s="3825">
         <v>3</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="s" s="3394">
+      <c r="A30" t="s" s="3826">
         <v>3</v>
       </c>
-      <c r="B30" t="s" s="3395">
+      <c r="B30" t="s" s="3827">
         <v>3</v>
       </c>
-      <c r="C30" t="s" s="3396">
+      <c r="C30" t="s" s="3828">
         <v>3</v>
       </c>
-      <c r="D30" t="s" s="3397">
+      <c r="D30" t="s" s="3829">
         <v>3</v>
       </c>
-      <c r="E30" t="s" s="3398">
+      <c r="E30" t="s" s="3830">
         <v>3</v>
       </c>
     </row>

</xml_diff>